<commit_message>
eliminato il test 14, fix errore WRONG_CLAIMS_ON_LOG sul test 11
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delprete\GitHub\it-fse-accreditamento\GATEWAY\A1#111SIEMENSHEALT\SIEMENS\RA2000\1.9.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7C929B-779B-42F3-BC0E-F1E83CDE36BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D457C755-7EC0-44B3-ABA4-AF83436D5847}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="196">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -644,12 +644,6 @@
     <t xml:space="preserve">4) Se il test NON è applicabile la colonna APPLICABILITA' riporterà NO e dovrà essere compilata esclusivamente la colonna RAZIONALE DI APPLICABILITA' con le motivazioni per cui il test non è applicabile </t>
   </si>
   <si>
-    <t>2b9b638f1c67a27e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.d2a3acd37b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>subject_application_vendor: SIEMENS</t>
   </si>
   <si>
@@ -657,18 +651,6 @@
   </si>
   <si>
     <t>subject_application_version: 1.9.2</t>
-  </si>
-  <si>
-    <t>2023-02-27T13:21:29.78Z</t>
-  </si>
-  <si>
-    <t>2023-02-27T14:40:50Z</t>
-  </si>
-  <si>
-    <t>597fa82ae1020d5d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.a2c2d22a8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-02-27T14:57:42Z</t>
@@ -866,9 +848,6 @@
     <t>SIEMENS</t>
   </si>
   <si>
-    <t>le sezioni non obbligatorie, Dicom, Storia Clinica, Suggerimenti per il medico prescrittore, non sono presenti nell'applicativo</t>
-  </si>
-  <si>
     <t>l'errore viene segnalato all'operatore</t>
   </si>
   <si>
@@ -882,6 +861,15 @@
   </si>
   <si>
     <t>nell'applicativo non sono presenti dati rigurado: conclusioni, i dati DICOM richiesti, la storia clinica del paziente, suggerimenti per il medico prescrittore</t>
+  </si>
+  <si>
+    <t>2023-03-14T10:21:30Z</t>
+  </si>
+  <si>
+    <t>1701154b589cd448</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.43a3bbdf18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3020,19 +3008,19 @@
   <dimension ref="A1:T880"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="26" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" style="26" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="26" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.28515625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="104.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.140625" style="26" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" style="26" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
@@ -3074,7 +3062,7 @@
       </c>
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D2" s="54"/>
       <c r="F2" s="27"/>
@@ -3099,7 +3087,7 @@
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="61" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" s="54"/>
       <c r="F3" s="27"/>
@@ -3122,7 +3110,7 @@
       <c r="A4" s="57"/>
       <c r="B4" s="58"/>
       <c r="C4" s="61" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="54"/>
       <c r="E4" s="30"/>
@@ -3146,7 +3134,7 @@
       <c r="A5" s="59"/>
       <c r="B5" s="60"/>
       <c r="C5" s="61" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D5" s="54"/>
       <c r="F5" s="27"/>
@@ -3284,7 +3272,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>11</v>
       </c>
@@ -3301,16 +3289,16 @@
         <v>30</v>
       </c>
       <c r="F10" s="39">
-        <v>44984</v>
+        <v>44999</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>125</v>
+        <v>193</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="J10" s="41" t="s">
         <v>40</v>
@@ -3354,7 +3342,7 @@
         <v>102</v>
       </c>
       <c r="K11" s="41" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
@@ -3392,7 +3380,7 @@
         <v>102</v>
       </c>
       <c r="K12" s="41" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
@@ -3406,7 +3394,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36">
         <v>14</v>
       </c>
@@ -3422,34 +3410,24 @@
       <c r="E13" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="39">
-        <v>44984</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="I13" s="40" t="s">
-        <v>128</v>
-      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="41"/>
+        <v>102</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>192</v>
+      </c>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
       <c r="N13" s="41"/>
       <c r="O13" s="41"/>
       <c r="P13" s="41"/>
-      <c r="Q13" s="41" t="s">
-        <v>100</v>
-      </c>
+      <c r="Q13" s="41"/>
       <c r="R13" s="44"/>
-      <c r="S13" s="42" t="s">
-        <v>194</v>
-      </c>
+      <c r="S13" s="42"/>
       <c r="T13" s="46" t="s">
         <v>110</v>
       </c>
@@ -3474,13 +3452,13 @@
         <v>44984</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J14" s="41" t="s">
         <v>40</v>
@@ -3493,13 +3471,13 @@
         <v>40</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="O14" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P14" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q14" s="41" t="s">
         <v>100</v>
@@ -3530,13 +3508,13 @@
         <v>44984</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J15" s="41" t="s">
         <v>40</v>
@@ -3549,13 +3527,13 @@
         <v>40</v>
       </c>
       <c r="N15" s="41" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="O15" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P15" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q15" s="41" t="s">
         <v>100</v>
@@ -3586,7 +3564,7 @@
         <v>44984</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H16" s="40"/>
       <c r="I16" s="40"/>
@@ -3605,7 +3583,7 @@
         <v>40</v>
       </c>
       <c r="P16" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q16" s="41" t="s">
         <v>100</v>
@@ -3618,7 +3596,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36">
         <v>75</v>
       </c>
@@ -3638,13 +3616,13 @@
         <v>44984</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J17" s="41" t="s">
         <v>40</v>
@@ -3657,13 +3635,13 @@
         <v>40</v>
       </c>
       <c r="N17" s="41" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="O17" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q17" s="41" t="s">
         <v>100</v>
@@ -3674,7 +3652,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36">
         <v>76</v>
       </c>
@@ -3694,13 +3672,13 @@
         <v>44984</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="J18" s="41" t="s">
         <v>40</v>
@@ -3713,13 +3691,13 @@
         <v>40</v>
       </c>
       <c r="N18" s="41" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="O18" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P18" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q18" s="41" t="s">
         <v>100</v>
@@ -3730,7 +3708,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36">
         <v>77</v>
       </c>
@@ -3750,13 +3728,13 @@
         <v>44985</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I19" s="40" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J19" s="41" t="s">
         <v>40</v>
@@ -3769,13 +3747,13 @@
         <v>40</v>
       </c>
       <c r="N19" s="41" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="O19" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P19" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q19" s="41" t="s">
         <v>100</v>
@@ -3786,7 +3764,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36">
         <v>78</v>
       </c>
@@ -3806,13 +3784,13 @@
         <v>44985</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H20" s="40" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J20" s="41" t="s">
         <v>40</v>
@@ -3825,13 +3803,13 @@
         <v>40</v>
       </c>
       <c r="N20" s="41" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="O20" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P20" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q20" s="41" t="s">
         <v>100</v>
@@ -3842,7 +3820,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36">
         <v>79</v>
       </c>
@@ -3862,13 +3840,13 @@
         <v>47908</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J21" s="41" t="s">
         <v>40</v>
@@ -3881,13 +3859,13 @@
         <v>40</v>
       </c>
       <c r="N21" s="41" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="O21" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P21" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q21" s="41" t="s">
         <v>100</v>
@@ -3898,7 +3876,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36">
         <v>80</v>
       </c>
@@ -3918,13 +3896,13 @@
         <v>47908</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H22" s="40" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I22" s="40" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J22" s="41" t="s">
         <v>40</v>
@@ -3937,13 +3915,13 @@
         <v>40</v>
       </c>
       <c r="N22" s="41" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="O22" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P22" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q22" s="41" t="s">
         <v>100</v>
@@ -3954,7 +3932,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36">
         <v>81</v>
       </c>
@@ -3974,13 +3952,13 @@
         <v>47908</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J23" s="41" t="s">
         <v>40</v>
@@ -3997,20 +3975,20 @@
         <v>40</v>
       </c>
       <c r="P23" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q23" s="41" t="s">
         <v>100</v>
       </c>
       <c r="R23" s="44"/>
       <c r="S23" s="42" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="T23" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="36">
         <v>82</v>
       </c>
@@ -4030,13 +4008,13 @@
         <v>47908</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J24" s="41" t="s">
         <v>40</v>
@@ -4053,14 +4031,14 @@
         <v>40</v>
       </c>
       <c r="P24" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q24" s="41" t="s">
         <v>100</v>
       </c>
       <c r="R24" s="44"/>
       <c r="S24" s="42" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="T24" s="46" t="s">
         <v>111</v>
@@ -4086,32 +4064,32 @@
         <v>47908</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J25" s="41" t="s">
         <v>40</v>
       </c>
       <c r="K25" s="41"/>
       <c r="L25" s="41" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="M25" s="41" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="N25" s="41" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="O25" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P25" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q25" s="41" t="s">
         <v>100</v>
@@ -4142,13 +4120,13 @@
         <v>47908</v>
       </c>
       <c r="G26" s="40" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J26" s="41" t="s">
         <v>40</v>
@@ -4161,13 +4139,13 @@
         <v>40</v>
       </c>
       <c r="N26" s="41" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O26" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P26" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q26" s="41" t="s">
         <v>100</v>
@@ -4178,7 +4156,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36">
         <v>85</v>
       </c>
@@ -4198,13 +4176,13 @@
         <v>47908</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J27" s="41" t="s">
         <v>40</v>
@@ -4217,13 +4195,13 @@
         <v>40</v>
       </c>
       <c r="N27" s="41" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="O27" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P27" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q27" s="41" t="s">
         <v>100</v>
@@ -4234,7 +4212,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
         <v>86</v>
       </c>
@@ -4254,13 +4232,13 @@
         <v>47908</v>
       </c>
       <c r="G28" s="40" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H28" s="40" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I28" s="40" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="J28" s="41" t="s">
         <v>40</v>
@@ -4273,13 +4251,13 @@
         <v>40</v>
       </c>
       <c r="N28" s="41" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O28" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P28" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q28" s="41" t="s">
         <v>100</v>
@@ -4310,13 +4288,13 @@
         <v>47908</v>
       </c>
       <c r="G29" s="40" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H29" s="40" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I29" s="40" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="J29" s="41" t="s">
         <v>40</v>
@@ -4329,13 +4307,13 @@
         <v>40</v>
       </c>
       <c r="N29" s="41" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="O29" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P29" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q29" s="41" t="s">
         <v>100</v>
@@ -4346,7 +4324,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>88</v>
       </c>
@@ -4370,7 +4348,7 @@
         <v>102</v>
       </c>
       <c r="K30" s="42" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
@@ -4383,7 +4361,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
         <v>89</v>
       </c>
@@ -4407,7 +4385,7 @@
         <v>102</v>
       </c>
       <c r="K31" s="42" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
@@ -4421,7 +4399,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
         <v>90</v>
       </c>
@@ -4445,7 +4423,7 @@
         <v>102</v>
       </c>
       <c r="K32" s="42" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
@@ -4459,7 +4437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
         <v>91</v>
       </c>
@@ -4483,7 +4461,7 @@
         <v>102</v>
       </c>
       <c r="K33" s="42" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
@@ -4497,7 +4475,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>92</v>
       </c>
@@ -4521,7 +4499,7 @@
         <v>102</v>
       </c>
       <c r="K34" s="42" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
@@ -4555,13 +4533,13 @@
         <v>47908</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H35" s="40" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J35" s="41" t="s">
         <v>40</v>
@@ -4574,13 +4552,13 @@
         <v>40</v>
       </c>
       <c r="N35" s="41" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="O35" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P35" s="41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Q35" s="41" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
integrata la report-checklist con maggiori dettagli richiesti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delprete\GitHub\it-fse-accreditamento\GATEWAY\A1#111SIEMENSHEALT\SIEMENS\RA2000\1.9.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D457C755-7EC0-44B3-ABA4-AF83436D5847}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2CCEB6-0E77-4581-8527-6E54DFE1FB4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="198">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -746,15 +746,6 @@
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]</t>
   </si>
   <si>
-    <t>2023-03-01T14:01:20Z</t>
-  </si>
-  <si>
-    <t>b342dd283db6bb1f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.c846804241^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>secondo la documentazione dovrebbe dare errore ma invece la risposta è 201</t>
   </si>
   <si>
@@ -774,9 +765,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.a5f5499dc2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>si</t>
   </si>
   <si>
     <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'code'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected.</t>
@@ -806,30 +794,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.bc92b1ddf6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>df4e03e054472614</t>
-  </si>
-  <si>
-    <t>2023-03-01T14:48:23Z</t>
-  </si>
-  <si>
-    <t>[ERRORE-b13| Sezione Precedenti Esami Eseguiti: La section deve contenere l'elemento 'text'.]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.2b4a4ea8e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-01T15:35:46Z</t>
-  </si>
-  <si>
-    <t>dd35455c82f435a9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.451e1bd8ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[ERRORE-b6| Il codice '10116451' non è corretto. La sezione deve essere valorizzata con uno dei seguenti codici:\n\t\t\t121181   Sezione DICOM Object Catalog\n\t\t\t18785-6  Sezione Quesito Diagnostico\n\t\t\t11329-0\t Sezione Storia Clinica\n\t\t\t55114-3\t Sezione Precedenti Esami Eseguiti\n\t\t\t55111-9\t Sezione Esame Eseguito\n\t\t\t18782-3\t Sezione Referto\n\t\t\t55110-1\t Sezione Conclusioni\n\t\t\t55107-7\t Sezione Informazioni Aggiuntive\n\t\t\t55109-3\t Sezione Complicanze\n\t\t\t18783-1  Sezione Suggerimenti per il medico prescrittore\n\t\t\t]</t>
-  </si>
-  <si>
     <t xml:space="preserve">i dati strutturati rigurado la "Storia Clinica" del paziente non sono presenti in RA2000 </t>
   </si>
   <si>
@@ -846,9 +810,6 @@
   </si>
   <si>
     <t>SIEMENS</t>
-  </si>
-  <si>
-    <t>l'errore viene segnalato all'operatore</t>
   </si>
   <si>
     <t>i dati strutturati rigurado la "Storia Clinica" del paziente non sono presenti nell'applicativo</t>
@@ -870,6 +831,51 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.43a3bbdf18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>non sono previsti dati rigurado participant/associatedEntity</t>
+  </si>
+  <si>
+    <t>Non sono presenti nell'applicativo i dati strutturati per compilare la sezione relativa gli esami precedenti</t>
+  </si>
+  <si>
+    <t>Non sono presenti nell'applicativo i dati strutturati per compilare la sezione relativa ai dati DICOM</t>
+  </si>
+  <si>
+    <t>i dati strutturati rigurado la "diagnosi sospettata" del paziente non sono presenti nell'applicativo</t>
+  </si>
+  <si>
+    <t>Connection to FSE gateway timeout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non è possibile che si verifichi in quanto sono parametri impostati in fase di configurazione   dell'applicativo.  La scelta se bloccare il flusso operativo del medico impedendo di proseguire l'attività, o se permettere la prosecuzione dell'attività e segnalare l'errore a gli operatori di backend è a discrezione dell'azienda opsedaliera. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La scelta se bloccare il flusso operativo del medico impedendo di proseguire l'attività, o se permettere la prosecuzione dell'attività e segnalare l'errore a gli operatori di backend è a discrezione dell'azienda opsedaliera. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La scelta se bloccare il flusso operativo del medico impedendo di proseguire l'attività, o se permettere la prosecuzione dell'attività e lasciare al backend la possibilità di ritentare l'invio è a discrezione dell'azienda opsedaliera. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il caso nella realtà non è possibile in quanto sono impostati in modo costante ed escluivo solo due vaolri V e N,  con valore di default N. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non è possibile che si verifichi in quanto nome e cognome del paziente sono dati obbligatori per inserire una posizione anagrafica nell'applicativo. </t>
+  </si>
+  <si>
+    <t>Non è possibile perché il campo prevedere obbligatoriamente i valori:  M,F,O che vengono mappati in modo fisso nei valori previsti dal CDA.</t>
+  </si>
+  <si>
+    <t>Non è possibile perché il campo prevede obbligatoriamente due valori  Normale o Urgente che vengono mappati in modo fisso nei valori previsti dal CDA.</t>
+  </si>
+  <si>
+    <t>Non è possibile perché il campo è obbligatorio per inserire un ordine nell'applicativo.</t>
+  </si>
+  <si>
+    <t>Non è possibile in quanto la valorizzazione è obbligatoria per poter chiudere un referto</t>
+  </si>
+  <si>
+    <t>L'applicativo prevede un valore di default RAD_PROG</t>
   </si>
 </sst>
 </file>
@@ -993,7 +999,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1010,6 +1016,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1371,7 +1383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1559,6 +1571,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3007,11 +3023,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T880"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="F34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,7 +3078,7 @@
       </c>
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D2" s="54"/>
       <c r="F2" s="27"/>
@@ -3272,7 +3288,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>11</v>
       </c>
@@ -3292,13 +3308,13 @@
         <v>44999</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="J10" s="41" t="s">
         <v>40</v>
@@ -3318,7 +3334,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36">
         <v>12</v>
       </c>
@@ -3342,7 +3358,7 @@
         <v>102</v>
       </c>
       <c r="K11" s="41" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
@@ -3356,7 +3372,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>13</v>
       </c>
@@ -3380,7 +3396,7 @@
         <v>102</v>
       </c>
       <c r="K12" s="41" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
@@ -3394,7 +3410,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36">
         <v>14</v>
       </c>
@@ -3418,7 +3434,7 @@
         <v>102</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
@@ -3432,7 +3448,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36">
         <v>31</v>
       </c>
@@ -3458,7 +3474,7 @@
         <v>124</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="J14" s="41" t="s">
         <v>40</v>
@@ -3488,7 +3504,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="36">
         <v>39</v>
       </c>
@@ -3514,7 +3530,7 @@
         <v>127</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="J15" s="41" t="s">
         <v>40</v>
@@ -3544,7 +3560,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="36">
         <v>47</v>
       </c>
@@ -3578,12 +3594,14 @@
       <c r="M16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="41"/>
+      <c r="N16" s="41" t="s">
+        <v>187</v>
+      </c>
       <c r="O16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="41" t="s">
-        <v>188</v>
+      <c r="P16" s="62" t="s">
+        <v>190</v>
       </c>
       <c r="Q16" s="41" t="s">
         <v>100</v>
@@ -3596,7 +3614,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="163.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36">
         <v>75</v>
       </c>
@@ -3641,7 +3659,7 @@
         <v>40</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q17" s="41" t="s">
         <v>100</v>
@@ -3652,7 +3670,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36">
         <v>76</v>
       </c>
@@ -3697,7 +3715,7 @@
         <v>40</v>
       </c>
       <c r="P18" s="41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q18" s="41" t="s">
         <v>100</v>
@@ -3708,7 +3726,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36">
         <v>77</v>
       </c>
@@ -3741,19 +3759,19 @@
       </c>
       <c r="K19" s="41"/>
       <c r="L19" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="M19" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="N19" s="41" t="s">
         <v>141</v>
       </c>
       <c r="O19" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P19" s="41" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="Q19" s="41" t="s">
         <v>100</v>
@@ -3764,7 +3782,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36">
         <v>78</v>
       </c>
@@ -3809,7 +3827,7 @@
         <v>40</v>
       </c>
       <c r="P20" s="41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q20" s="41" t="s">
         <v>100</v>
@@ -3820,7 +3838,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36">
         <v>79</v>
       </c>
@@ -3865,7 +3883,7 @@
         <v>40</v>
       </c>
       <c r="P21" s="41" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="Q21" s="41" t="s">
         <v>100</v>
@@ -3876,7 +3894,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36">
         <v>80</v>
       </c>
@@ -3909,19 +3927,19 @@
       </c>
       <c r="K22" s="41"/>
       <c r="L22" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="M22" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="N22" s="41" t="s">
         <v>153</v>
       </c>
       <c r="O22" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P22" s="41" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="Q22" s="41" t="s">
         <v>100</v>
@@ -3932,7 +3950,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36">
         <v>81</v>
       </c>
@@ -3948,47 +3966,29 @@
       <c r="E23" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="39">
-        <v>47908</v>
-      </c>
-      <c r="G23" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="H23" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="I23" s="40" t="s">
-        <v>156</v>
-      </c>
+      <c r="F23" s="39"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
       <c r="J23" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="M23" s="41" t="s">
-        <v>102</v>
-      </c>
+      <c r="K23" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
       <c r="N23" s="41"/>
-      <c r="O23" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="P23" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q23" s="41" t="s">
-        <v>100</v>
-      </c>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
       <c r="R23" s="44"/>
-      <c r="S23" s="42" t="s">
-        <v>157</v>
-      </c>
+      <c r="S23" s="42"/>
       <c r="T23" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="36">
         <v>82</v>
       </c>
@@ -4008,13 +4008,13 @@
         <v>47908</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J24" s="41" t="s">
         <v>40</v>
@@ -4028,17 +4028,17 @@
       </c>
       <c r="N24" s="41"/>
       <c r="O24" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P24" s="41" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="Q24" s="41" t="s">
         <v>100</v>
       </c>
       <c r="R24" s="44"/>
       <c r="S24" s="42" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="T24" s="46" t="s">
         <v>111</v>
@@ -4064,32 +4064,32 @@
         <v>47908</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J25" s="41" t="s">
         <v>40</v>
       </c>
       <c r="K25" s="41"/>
       <c r="L25" s="41" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="M25" s="41" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="N25" s="41" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O25" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P25" s="41" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="Q25" s="41" t="s">
         <v>100</v>
@@ -4120,13 +4120,13 @@
         <v>47908</v>
       </c>
       <c r="G26" s="40" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J26" s="41" t="s">
         <v>40</v>
@@ -4139,13 +4139,13 @@
         <v>40</v>
       </c>
       <c r="N26" s="41" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O26" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P26" s="41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q26" s="41" t="s">
         <v>100</v>
@@ -4156,7 +4156,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36">
         <v>85</v>
       </c>
@@ -4176,32 +4176,32 @@
         <v>47908</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J27" s="41" t="s">
         <v>40</v>
       </c>
       <c r="K27" s="41"/>
       <c r="L27" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="M27" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="N27" s="41" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="O27" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P27" s="41" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="Q27" s="41" t="s">
         <v>100</v>
@@ -4212,7 +4212,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
         <v>86</v>
       </c>
@@ -4228,47 +4228,29 @@
       <c r="E28" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="39">
-        <v>47908</v>
-      </c>
-      <c r="G28" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="H28" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="I28" s="40" t="s">
-        <v>177</v>
-      </c>
+      <c r="F28" s="39"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
       <c r="J28" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="N28" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="O28" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="P28" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q28" s="41" t="s">
-        <v>100</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="K28" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
       <c r="R28" s="44"/>
       <c r="S28" s="42"/>
       <c r="T28" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="36">
         <v>87</v>
       </c>
@@ -4284,47 +4266,29 @@
       <c r="E29" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="39">
-        <v>47908</v>
-      </c>
-      <c r="G29" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="H29" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="I29" s="40" t="s">
-        <v>180</v>
-      </c>
+      <c r="F29" s="39"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
       <c r="J29" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="M29" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="N29" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="O29" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="P29" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q29" s="41" t="s">
-        <v>100</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="K29" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
       <c r="R29" s="44"/>
       <c r="S29" s="42"/>
       <c r="T29" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>88</v>
       </c>
@@ -4348,7 +4312,7 @@
         <v>102</v>
       </c>
       <c r="K30" s="42" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
@@ -4361,7 +4325,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
         <v>89</v>
       </c>
@@ -4385,7 +4349,7 @@
         <v>102</v>
       </c>
       <c r="K31" s="42" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
@@ -4399,7 +4363,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
         <v>90</v>
       </c>
@@ -4423,7 +4387,7 @@
         <v>102</v>
       </c>
       <c r="K32" s="42" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
@@ -4437,7 +4401,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
         <v>91</v>
       </c>
@@ -4461,7 +4425,7 @@
         <v>102</v>
       </c>
       <c r="K33" s="42" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
@@ -4475,7 +4439,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>92</v>
       </c>
@@ -4499,7 +4463,7 @@
         <v>102</v>
       </c>
       <c r="K34" s="42" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
@@ -4533,32 +4497,32 @@
         <v>47908</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="H35" s="40" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="J35" s="41" t="s">
         <v>40</v>
       </c>
       <c r="K35" s="41"/>
       <c r="L35" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="M35" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="N35" s="41" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="O35" s="41" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P35" s="41" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="Q35" s="41" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
aggiornata la report-check list con le indicazioni ricevute via mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delprete\GitHub\it-fse-accreditamento\GATEWAY\A1#111SIEMENSHEALT\SIEMENS\RA2000\1.9.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2CCEB6-0E77-4581-8527-6E54DFE1FB4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD3505C-D711-48BC-B9B9-8FB0C597C323}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="Summary" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$35</definedName>
   </definedNames>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="206">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -833,15 +836,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.43a3bbdf18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>non sono previsti dati rigurado participant/associatedEntity</t>
-  </si>
-  <si>
-    <t>Non sono presenti nell'applicativo i dati strutturati per compilare la sezione relativa gli esami precedenti</t>
-  </si>
-  <si>
-    <t>Non sono presenti nell'applicativo i dati strutturati per compilare la sezione relativa ai dati DICOM</t>
-  </si>
-  <si>
     <t>i dati strutturati rigurado la "diagnosi sospettata" del paziente non sono presenti nell'applicativo</t>
   </si>
   <si>
@@ -876,6 +870,39 @@
   </si>
   <si>
     <t>L'applicativo prevede un valore di default RAD_PROG</t>
+  </si>
+  <si>
+    <t>2023-03-01T14:01:20Z</t>
+  </si>
+  <si>
+    <t>b342dd283db6bb1f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.c846804241^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-01T14:48:23Z</t>
+  </si>
+  <si>
+    <t>df4e03e054472614</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.2b4a4ea8e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-b13| Sezione Precedenti Esami Eseguiti: La section deve contenere l'elemento 'text'.]</t>
+  </si>
+  <si>
+    <t>2023-03-01T15:35:46Z</t>
+  </si>
+  <si>
+    <t>dd35455c82f435a9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.451e1bd8ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-b6| Il codice '10116451' non è corretto. La sezione deve essere valorizzata con uno dei seguenti codici:\n\t\t\t121181   Sezione DICOM Object Catalog\n\t\t\t18785-6  Sezione Quesito Diagnostico\n\t\t\t11329-0\t Sezione Storia Clinica\n\t\t\t55114-3\t Sezione Precedenti Esami Eseguiti\n\t\t\t55111-9\t Sezione Esame Eseguito\n\t\t\t18782-3\t Sezione Referto\n\t\t\t55110-1\t Sezione Conclusioni\n\t\t\t55107-7\t Sezione Informazioni Aggiuntive\n\t\t\t55109-3\t Sezione Complicanze\n\t\t\t18783-1  Sezione Suggerimenti per il medico prescrittore\n\t\t\t]</t>
   </si>
 </sst>
 </file>
@@ -1522,6 +1549,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1571,10 +1602,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1652,6 +1679,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="TestCases-ok"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3023,11 +3065,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T880"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F34" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,14 +3115,14 @@
       <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="55"/>
       <c r="F2" s="27"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
@@ -3098,14 +3140,14 @@
       <c r="T2" s="28"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="61" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="54"/>
+      <c r="D3" s="55"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
@@ -3123,12 +3165,12 @@
       <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="61" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="30"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
@@ -3147,12 +3189,12 @@
       <c r="T4" s="28"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61" t="s">
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
@@ -3170,8 +3212,8 @@
       <c r="T5" s="28"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="32"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -3288,7 +3330,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>11</v>
       </c>
@@ -3334,7 +3376,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36">
         <v>12</v>
       </c>
@@ -3372,7 +3414,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>13</v>
       </c>
@@ -3410,7 +3452,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36">
         <v>14</v>
       </c>
@@ -3493,7 +3535,7 @@
         <v>40</v>
       </c>
       <c r="P14" s="41" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Q14" s="41" t="s">
         <v>100</v>
@@ -3549,7 +3591,7 @@
         <v>40</v>
       </c>
       <c r="P15" s="41" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Q15" s="41" t="s">
         <v>100</v>
@@ -3595,13 +3637,13 @@
         <v>40</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="62" t="s">
-        <v>190</v>
+      <c r="P16" s="49" t="s">
+        <v>187</v>
       </c>
       <c r="Q16" s="41" t="s">
         <v>100</v>
@@ -3659,7 +3701,7 @@
         <v>40</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q17" s="41" t="s">
         <v>100</v>
@@ -3715,7 +3757,7 @@
         <v>40</v>
       </c>
       <c r="P18" s="41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q18" s="41" t="s">
         <v>100</v>
@@ -3771,7 +3813,7 @@
         <v>102</v>
       </c>
       <c r="P19" s="41" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Q19" s="41" t="s">
         <v>100</v>
@@ -3827,7 +3869,7 @@
         <v>40</v>
       </c>
       <c r="P20" s="41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q20" s="41" t="s">
         <v>100</v>
@@ -3883,7 +3925,7 @@
         <v>40</v>
       </c>
       <c r="P21" s="41" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Q21" s="41" t="s">
         <v>100</v>
@@ -3939,7 +3981,7 @@
         <v>102</v>
       </c>
       <c r="P22" s="41" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="Q22" s="41" t="s">
         <v>100</v>
@@ -3950,7 +3992,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36">
         <v>81</v>
       </c>
@@ -3966,24 +4008,42 @@
       <c r="E23" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
+      <c r="F23" s="39">
+        <v>47908</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="I23" s="40" t="s">
+        <v>197</v>
+      </c>
       <c r="J23" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="K23" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
+      <c r="M23" s="41" t="s">
+        <v>102</v>
+      </c>
       <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
+      <c r="O23" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="P23" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q23" s="41" t="s">
+        <v>100</v>
+      </c>
       <c r="R23" s="44"/>
-      <c r="S23" s="42"/>
+      <c r="S23" s="42" t="s">
+        <v>154</v>
+      </c>
       <c r="T23" s="46" t="s">
         <v>111</v>
       </c>
@@ -4031,7 +4091,7 @@
         <v>102</v>
       </c>
       <c r="P24" s="41" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Q24" s="41" t="s">
         <v>100</v>
@@ -4089,7 +4149,7 @@
         <v>102</v>
       </c>
       <c r="P25" s="41" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Q25" s="41" t="s">
         <v>100</v>
@@ -4145,7 +4205,7 @@
         <v>40</v>
       </c>
       <c r="P26" s="41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q26" s="41" t="s">
         <v>100</v>
@@ -4201,7 +4261,7 @@
         <v>102</v>
       </c>
       <c r="P27" s="41" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q27" s="41" t="s">
         <v>100</v>
@@ -4212,7 +4272,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
         <v>86</v>
       </c>
@@ -4228,29 +4288,47 @@
       <c r="E28" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
+      <c r="F28" s="39">
+        <v>47908</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="I28" s="40" t="s">
+        <v>200</v>
+      </c>
       <c r="J28" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="K28" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
+      <c r="M28" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="N28" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="O28" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="P28" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q28" s="41" t="s">
+        <v>100</v>
+      </c>
       <c r="R28" s="44"/>
       <c r="S28" s="42"/>
       <c r="T28" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="36">
         <v>87</v>
       </c>
@@ -4266,29 +4344,47 @@
       <c r="E29" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="39"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
+      <c r="F29" s="39">
+        <v>47908</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>204</v>
+      </c>
       <c r="J29" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="K29" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
+      <c r="M29" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="N29" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="O29" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="P29" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q29" s="41" t="s">
+        <v>100</v>
+      </c>
       <c r="R29" s="44"/>
       <c r="S29" s="42"/>
       <c r="T29" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>88</v>
       </c>
@@ -4325,7 +4421,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
         <v>89</v>
       </c>
@@ -4363,7 +4459,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
         <v>90</v>
       </c>
@@ -4401,7 +4497,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
         <v>91</v>
       </c>
@@ -4463,7 +4559,7 @@
         <v>102</v>
       </c>
       <c r="K34" s="42" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
@@ -4522,7 +4618,7 @@
         <v>102</v>
       </c>
       <c r="P35" s="41" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q35" s="41" t="s">
         <v>100</v>
@@ -18914,7 +19010,7 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7251B2DD-EAA3-474F-9C39-00147BB6DBBD}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
@@ -18925,13 +19021,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10:J35</xm:sqref>
+          <xm:sqref>J10:J28 J30:J35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>Q10:Q35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{F579B62E-3466-4E25-95F3-15FCB01CCA6C}">
+          <x14:formula1>
+            <xm:f>'C:\Users\delprete\Ricoh Europe PLC\EU-NPO-RIS - Siemens - client-FSE\test-fse\storia-accreditamento\A1#111SIEMENSHEALT_accreditamento\SIEMENS\RA2000\1.9.2\[report-checklist-accreditamento-work.xlsx]Sheet1'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>J29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
corretti test 81,82 come da mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIEMENSHEALT/SIEMENS/RA2000/1.9.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delprete\GitHub\it-fse-accreditamento\GATEWAY\A1#111SIEMENSHEALT\SIEMENS\RA2000\1.9.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD3505C-D711-48BC-B9B9-8FB0C597C323}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7279D8-7631-40B9-8138-45D52125E840}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="208">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -749,18 +749,6 @@
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]</t>
   </si>
   <si>
-    <t>secondo la documentazione dovrebbe dare errore ma invece la risposta è 201</t>
-  </si>
-  <si>
-    <t>2023-03-01T14:04:58Z</t>
-  </si>
-  <si>
-    <t>5108a885bfa642e9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.a7c1f7bf5d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-03-01T14:13:57Z</t>
   </si>
   <si>
@@ -860,9 +848,6 @@
     <t>Non è possibile perché il campo prevedere obbligatoriamente i valori:  M,F,O che vengono mappati in modo fisso nei valori previsti dal CDA.</t>
   </si>
   <si>
-    <t>Non è possibile perché il campo prevede obbligatoriamente due valori  Normale o Urgente che vengono mappati in modo fisso nei valori previsti dal CDA.</t>
-  </si>
-  <si>
     <t>Non è possibile perché il campo è obbligatorio per inserire un ordine nell'applicativo.</t>
   </si>
   <si>
@@ -870,15 +855,6 @@
   </si>
   <si>
     <t>L'applicativo prevede un valore di default RAD_PROG</t>
-  </si>
-  <si>
-    <t>2023-03-01T14:01:20Z</t>
-  </si>
-  <si>
-    <t>b342dd283db6bb1f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.c846804241^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-03-01T14:48:23Z</t>
@@ -903,6 +879,36 @@
   </si>
   <si>
     <t>[ERRORE-b6| Il codice '10116451' non è corretto. La sezione deve essere valorizzata con uno dei seguenti codici:\n\t\t\t121181   Sezione DICOM Object Catalog\n\t\t\t18785-6  Sezione Quesito Diagnostico\n\t\t\t11329-0\t Sezione Storia Clinica\n\t\t\t55114-3\t Sezione Precedenti Esami Eseguiti\n\t\t\t55111-9\t Sezione Esame Eseguito\n\t\t\t18782-3\t Sezione Referto\n\t\t\t55110-1\t Sezione Conclusioni\n\t\t\t55107-7\t Sezione Informazioni Aggiuntive\n\t\t\t55109-3\t Sezione Complicanze\n\t\t\t18783-1  Sezione Suggerimenti per il medico prescrittore\n\t\t\t]</t>
+  </si>
+  <si>
+    <t>2023-03-31T16:30:49Z</t>
+  </si>
+  <si>
+    <t>d5c8a21762be82bb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.ccdc8df64a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.2.7 v1.0.0, Codes: 9999]</t>
+  </si>
+  <si>
+    <t>Non è possibile in quanto il codice è impostato nella configurazione dell'applicativo</t>
+  </si>
+  <si>
+    <t>2023-04-03T11:47:23Z</t>
+  </si>
+  <si>
+    <t>a76abb64de7c74c0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.65951697ec342cfcc022dbde15319a69ef7b23463829fa9ff9f7207b5188076b.31c6b06a77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-39| inFulfillmentOf\/order\/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]</t>
+  </si>
+  <si>
+    <t>Non è possibile perché il campo prevede obbligatoriamente due valori  Normale o Urgente che vengono mappati in modo fisso nei valori previsti (R,UR).</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1553,6 +1559,38 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -3065,11 +3103,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T880"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
+      <selection pane="bottomRight" activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,14 +3153,14 @@
       <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="55"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="64"/>
       <c r="F2" s="27"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
@@ -3140,14 +3178,14 @@
       <c r="T2" s="28"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="62" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="64"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
@@ -3165,12 +3203,12 @@
       <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="62" t="s">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="30"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
@@ -3189,12 +3227,12 @@
       <c r="T4" s="28"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="62" t="s">
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="64"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
@@ -3212,8 +3250,8 @@
       <c r="T5" s="28"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="32"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -3330,7 +3368,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>11</v>
       </c>
@@ -3350,13 +3388,13 @@
         <v>44999</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J10" s="41" t="s">
         <v>40</v>
@@ -3376,7 +3414,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36">
         <v>12</v>
       </c>
@@ -3400,7 +3438,7 @@
         <v>102</v>
       </c>
       <c r="K11" s="41" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
@@ -3414,7 +3452,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>13</v>
       </c>
@@ -3438,7 +3476,7 @@
         <v>102</v>
       </c>
       <c r="K12" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
@@ -3452,7 +3490,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36">
         <v>14</v>
       </c>
@@ -3476,7 +3514,7 @@
         <v>102</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
@@ -3516,7 +3554,7 @@
         <v>124</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J14" s="41" t="s">
         <v>40</v>
@@ -3535,7 +3573,7 @@
         <v>40</v>
       </c>
       <c r="P14" s="41" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="Q14" s="41" t="s">
         <v>100</v>
@@ -3572,7 +3610,7 @@
         <v>127</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J15" s="41" t="s">
         <v>40</v>
@@ -3591,7 +3629,7 @@
         <v>40</v>
       </c>
       <c r="P15" s="41" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="Q15" s="41" t="s">
         <v>100</v>
@@ -3637,13 +3675,13 @@
         <v>40</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="O16" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P16" s="49" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="Q16" s="41" t="s">
         <v>100</v>
@@ -3701,7 +3739,7 @@
         <v>40</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q17" s="41" t="s">
         <v>100</v>
@@ -3712,7 +3750,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36">
         <v>76</v>
       </c>
@@ -3757,7 +3795,7 @@
         <v>40</v>
       </c>
       <c r="P18" s="41" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q18" s="41" t="s">
         <v>100</v>
@@ -3768,7 +3806,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36">
         <v>77</v>
       </c>
@@ -3813,7 +3851,7 @@
         <v>102</v>
       </c>
       <c r="P19" s="41" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="Q19" s="41" t="s">
         <v>100</v>
@@ -3869,7 +3907,7 @@
         <v>40</v>
       </c>
       <c r="P20" s="41" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q20" s="41" t="s">
         <v>100</v>
@@ -3880,7 +3918,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36">
         <v>79</v>
       </c>
@@ -3925,7 +3963,7 @@
         <v>40</v>
       </c>
       <c r="P21" s="41" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="Q21" s="41" t="s">
         <v>100</v>
@@ -3936,7 +3974,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36">
         <v>80</v>
       </c>
@@ -3981,7 +4019,7 @@
         <v>102</v>
       </c>
       <c r="P22" s="41" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="Q22" s="41" t="s">
         <v>100</v>
@@ -3992,7 +4030,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36">
         <v>81</v>
       </c>
@@ -4009,16 +4047,16 @@
         <v>60</v>
       </c>
       <c r="F23" s="39">
-        <v>47908</v>
+        <v>44957</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J23" s="41" t="s">
         <v>40</v>
@@ -4030,77 +4068,77 @@
       <c r="M23" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="N23" s="41"/>
+      <c r="N23" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="O23" s="41" t="s">
         <v>102</v>
       </c>
       <c r="P23" s="41" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="Q23" s="41" t="s">
         <v>100</v>
       </c>
       <c r="R23" s="44"/>
-      <c r="S23" s="42" t="s">
-        <v>154</v>
-      </c>
+      <c r="S23" s="42"/>
       <c r="T23" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36">
+    <row r="24" spans="1:20" s="58" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="50">
         <v>82</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="39">
-        <v>47908</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="H24" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="I24" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="J24" s="41" t="s">
+      <c r="F24" s="53">
+        <v>45019</v>
+      </c>
+      <c r="G24" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="H24" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="I24" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="J24" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41" t="s">
+      <c r="K24" s="49"/>
+      <c r="L24" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41" t="s">
+      <c r="N24" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="O24" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="P24" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q24" s="41" t="s">
+      <c r="P24" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q24" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="R24" s="44"/>
-      <c r="S24" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="T24" s="46" t="s">
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
+      <c r="T24" s="57" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4124,13 +4162,13 @@
         <v>47908</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J25" s="41" t="s">
         <v>40</v>
@@ -4143,13 +4181,13 @@
         <v>102</v>
       </c>
       <c r="N25" s="41" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O25" s="41" t="s">
         <v>102</v>
       </c>
       <c r="P25" s="41" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Q25" s="41" t="s">
         <v>100</v>
@@ -4180,13 +4218,13 @@
         <v>47908</v>
       </c>
       <c r="G26" s="40" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J26" s="41" t="s">
         <v>40</v>
@@ -4199,13 +4237,13 @@
         <v>40</v>
       </c>
       <c r="N26" s="41" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O26" s="41" t="s">
         <v>40</v>
       </c>
       <c r="P26" s="41" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q26" s="41" t="s">
         <v>100</v>
@@ -4216,7 +4254,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36">
         <v>85</v>
       </c>
@@ -4236,13 +4274,13 @@
         <v>47908</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J27" s="41" t="s">
         <v>40</v>
@@ -4255,13 +4293,13 @@
         <v>102</v>
       </c>
       <c r="N27" s="41" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="O27" s="41" t="s">
         <v>102</v>
       </c>
       <c r="P27" s="41" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Q27" s="41" t="s">
         <v>100</v>
@@ -4272,7 +4310,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
         <v>86</v>
       </c>
@@ -4292,13 +4330,13 @@
         <v>47908</v>
       </c>
       <c r="G28" s="40" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="H28" s="40" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I28" s="40" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="J28" s="41" t="s">
         <v>40</v>
@@ -4311,13 +4349,13 @@
         <v>102</v>
       </c>
       <c r="N28" s="41" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="O28" s="41" t="s">
         <v>102</v>
       </c>
       <c r="P28" s="41" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q28" s="41" t="s">
         <v>100</v>
@@ -4348,13 +4386,13 @@
         <v>47908</v>
       </c>
       <c r="G29" s="40" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H29" s="40" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I29" s="40" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="J29" s="41" t="s">
         <v>40</v>
@@ -4367,13 +4405,13 @@
         <v>102</v>
       </c>
       <c r="N29" s="41" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="O29" s="41" t="s">
         <v>102</v>
       </c>
       <c r="P29" s="41" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q29" s="41" t="s">
         <v>100</v>
@@ -4384,7 +4422,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>88</v>
       </c>
@@ -4408,7 +4446,7 @@
         <v>102</v>
       </c>
       <c r="K30" s="42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
@@ -4421,7 +4459,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
         <v>89</v>
       </c>
@@ -4445,7 +4483,7 @@
         <v>102</v>
       </c>
       <c r="K31" s="42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
@@ -4459,7 +4497,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
         <v>90</v>
       </c>
@@ -4483,7 +4521,7 @@
         <v>102</v>
       </c>
       <c r="K32" s="42" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
@@ -4497,7 +4535,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
         <v>91</v>
       </c>
@@ -4521,7 +4559,7 @@
         <v>102</v>
       </c>
       <c r="K33" s="42" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
@@ -4535,7 +4573,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>92</v>
       </c>
@@ -4559,7 +4597,7 @@
         <v>102</v>
       </c>
       <c r="K34" s="42" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
@@ -4573,7 +4611,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="36">
         <v>93</v>
       </c>
@@ -4593,13 +4631,13 @@
         <v>47908</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H35" s="40" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J35" s="41" t="s">
         <v>40</v>
@@ -4612,13 +4650,13 @@
         <v>102</v>
       </c>
       <c r="N35" s="41" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="O35" s="41" t="s">
         <v>102</v>
       </c>
       <c r="P35" s="41" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="Q35" s="41" t="s">
         <v>100</v>

</xml_diff>